<commit_message>
New run + Updated statistics
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mj115gl\work_dir\thesis\audio-semantics\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A849BEA-6E1B-4CCE-8243-9F42182577C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA585B74-0C4F-4454-8F18-697CD0510E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{FEFB47C1-2158-4964-8BE6-472CD43CBB76}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
   <si>
     <t>Level 1</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>Original</t>
+  </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t>Avg tokens in word</t>
+  </si>
+  <si>
+    <t>Clusters</t>
+  </si>
+  <si>
+    <t>Cluster threshold</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -235,15 +247,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -359,17 +362,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,62 +407,79 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -446,28 +488,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -476,25 +503,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -811,16 +863,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB4473A-7175-4429-BDCF-232E357ED7DB}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="10" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -829,29 +881,29 @@
       <c r="A2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="46" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="46" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="46" t="s">
+      <c r="H2" s="22"/>
+      <c r="I2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="47"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="43"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
@@ -872,13 +924,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -896,9 +948,9 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="28"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
@@ -914,372 +966,654 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="3" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11">
+      <c r="E6" s="19"/>
+      <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11">
+      <c r="G6" s="19"/>
+      <c r="H6" s="7">
         <v>5</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="22" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="28">
+        <v>0.45</v>
+      </c>
+      <c r="F7" s="51"/>
+      <c r="G7" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="H7" s="51"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="46">
+        <v>748</v>
+      </c>
+      <c r="F8" s="47"/>
+      <c r="G8" s="46">
+        <v>19619</v>
+      </c>
+      <c r="H8" s="47"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="50"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="28">
+        <v>1.7788999999999999</v>
+      </c>
+      <c r="F9" s="51"/>
+      <c r="G9" s="28">
+        <v>3.6576</v>
+      </c>
+      <c r="H9" s="51"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E10" s="25">
         <v>9.6433999999999997</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="22">
+      <c r="F10" s="26"/>
+      <c r="G10" s="25">
         <v>-3.9738000000000002</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="17" t="s">
+      <c r="H10" s="26"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E11" s="30">
         <v>0.4148</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="26">
+      <c r="F11" s="31"/>
+      <c r="G11" s="30">
         <v>1.5122</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
+      <c r="H11" s="31"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36">
         <v>2</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B12" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D12" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E12" s="17">
         <v>20000</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="20">
+      <c r="F12" s="18"/>
+      <c r="G12" s="17">
         <v>20000</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="20">
+      <c r="H12" s="18"/>
+      <c r="I12" s="17">
         <v>50000</v>
       </c>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="2" t="s">
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7">
+      <c r="E13" s="6"/>
+      <c r="F13" s="7">
         <v>250</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7">
+      <c r="G13" s="6"/>
+      <c r="H13" s="7">
         <v>150</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7">
+      <c r="I13" s="6"/>
+      <c r="J13" s="7">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="3" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11">
+      <c r="E14" s="19"/>
+      <c r="F14" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11">
+      <c r="G14" s="19"/>
+      <c r="H14" s="7">
         <v>5</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="11">
+      <c r="I14" s="19"/>
+      <c r="J14" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="22" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0.45</v>
+      </c>
+      <c r="F15" s="51"/>
+      <c r="G15" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="H15" s="51"/>
+      <c r="I15" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="J15" s="51"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="46">
+        <v>1138</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="46">
+        <v>19615</v>
+      </c>
+      <c r="H16" s="47"/>
+      <c r="I16" s="46">
+        <v>49506</v>
+      </c>
+      <c r="J16" s="47"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="28">
+        <v>1.8855999999999999</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="28">
+        <v>3.8527999999999998</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="28">
+        <v>3.2311999999999999</v>
+      </c>
+      <c r="J17" s="51"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="49">
+      <c r="E18" s="32">
         <v>10.0322</v>
       </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="22">
+      <c r="F18" s="33"/>
+      <c r="G18" s="25">
         <v>8.7571999999999992</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="22">
+      <c r="H18" s="26"/>
+      <c r="I18" s="25">
         <v>2.8107000000000002</v>
       </c>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="17" t="s">
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E19" s="30">
         <v>9.579E-2</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="26">
+      <c r="F19" s="31"/>
+      <c r="G19" s="30">
         <v>0.27729999999999999</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="40">
+      <c r="H19" s="31"/>
+      <c r="I19" s="34">
         <v>-4.0624000000000002</v>
       </c>
-      <c r="J13" s="41"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
+      <c r="J19" s="35"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
         <v>3</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B20" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E20" s="6">
         <v>20000</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="6">
+      <c r="F20" s="7"/>
+      <c r="G20" s="6">
         <v>60000</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="2" t="s">
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7">
+      <c r="E21" s="6"/>
+      <c r="F21" s="7">
         <v>150</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="7">
+      <c r="G21" s="6"/>
+      <c r="H21" s="7">
         <v>250</v>
       </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="3" t="s">
+      <c r="I21" s="8"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11">
+      <c r="E22" s="19"/>
+      <c r="F22" s="7">
         <v>1</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11">
+      <c r="G22" s="19"/>
+      <c r="H22" s="7">
         <v>5</v>
       </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="22" t="s">
+      <c r="I22" s="8"/>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="28">
+        <v>0.45</v>
+      </c>
+      <c r="F23" s="51"/>
+      <c r="G23" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="H23" s="51"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="46">
+        <v>418</v>
+      </c>
+      <c r="F24" s="47"/>
+      <c r="G24" s="46">
+        <v>56607</v>
+      </c>
+      <c r="H24" s="47"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="50"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="28">
+        <v>3.0828000000000002</v>
+      </c>
+      <c r="F25" s="51"/>
+      <c r="G25" s="28">
+        <v>3.0446</v>
+      </c>
+      <c r="H25" s="51"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D26" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E26" s="44">
         <v>11.2354</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="22">
+      <c r="F26" s="45"/>
+      <c r="G26" s="25">
         <v>8.9542999999999999</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="17" t="s">
+      <c r="H26" s="26"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="29"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E27" s="30">
         <v>-3.0592000000000001</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="26">
+      <c r="F27" s="31"/>
+      <c r="G27" s="30">
         <v>0.20230000000000001</v>
       </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="25"/>
-    </row>
+      <c r="H27" s="31"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27">
+        <v>4</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="19">
+        <v>60000</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="27"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="7">
+        <v>250</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="28">
+        <v>0.95</v>
+      </c>
+      <c r="F31" s="51"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="27"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="46">
+        <v>56497</v>
+      </c>
+      <c r="F32" s="47"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="50"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="28">
+        <v>1.7931999999999999</v>
+      </c>
+      <c r="F33" s="51"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="27"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="32">
+        <v>9.0103000000000009</v>
+      </c>
+      <c r="F34" s="33"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="29"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="30">
+        <v>1.0289999999999999</v>
+      </c>
+      <c r="F35" s="31"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="72">
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="B28:B35"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="B20:B27"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New runs with same-word ABX test
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mj115gl\work_dir\thesis\audio-semantics\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1418121D-7EFC-4A48-9948-9CA543B9971E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746BCD8C-0352-41DC-845A-E90A5B95CCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{FEFB47C1-2158-4964-8BE6-472CD43CBB76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FEFB47C1-2158-4964-8BE6-472CD43CBB76}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Model Configs" sheetId="3" r:id="rId1"/>
+    <sheet name="Configs" sheetId="1" r:id="rId2"/>
+    <sheet name="Results" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="82">
   <si>
     <t>Level 1</t>
   </si>
@@ -163,6 +165,123 @@
   </si>
   <si>
     <t>Compressed</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>ABX Score</t>
+  </si>
+  <si>
+    <t>Baseline - Sparse vectors</t>
+  </si>
+  <si>
+    <t>Kind</t>
+  </si>
+  <si>
+    <t>Similarity Score</t>
+  </si>
+  <si>
+    <t>comp</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>levelwise</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>Audio process</t>
+  </si>
+  <si>
+    <t>CPC</t>
+  </si>
+  <si>
+    <t>Combined</t>
+  </si>
+  <si>
+    <t>level0 sp</t>
+  </si>
+  <si>
+    <t>level0 w2v window</t>
+  </si>
+  <si>
+    <t>level0 w2v vs</t>
+  </si>
+  <si>
+    <t>level1 sp</t>
+  </si>
+  <si>
+    <t>level1 w2v vs</t>
+  </si>
+  <si>
+    <t>level1 w2v window</t>
+  </si>
+  <si>
+    <t>level2 sp</t>
+  </si>
+  <si>
+    <t>level2 w2v vs</t>
+  </si>
+  <si>
+    <t>level2 w2v window</t>
+  </si>
+  <si>
+    <t>db vs</t>
+  </si>
+  <si>
+    <t>db max_len</t>
+  </si>
+  <si>
+    <t>bert</t>
+  </si>
+  <si>
+    <t>tokeniser</t>
+  </si>
+  <si>
+    <t>sp-unigram</t>
+  </si>
+  <si>
+    <t>vec-model</t>
+  </si>
+  <si>
+    <t>word2vec</t>
+  </si>
+  <si>
+    <t>fasttext</t>
+  </si>
+  <si>
+    <t>additional 1</t>
+  </si>
+  <si>
+    <t>additional 2</t>
+  </si>
+  <si>
+    <t>additional 3</t>
+  </si>
+  <si>
+    <t>additional 4</t>
+  </si>
+  <si>
+    <t>additional 5</t>
+  </si>
+  <si>
+    <t>additional 6</t>
+  </si>
+  <si>
+    <t>sparse</t>
+  </si>
+  <si>
+    <t>tf-idf</t>
+  </si>
+  <si>
+    <t>ABX Score (SAME WORD)</t>
+  </si>
+  <si>
+    <t>Mixed</t>
   </si>
 </sst>
 </file>
@@ -172,7 +291,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +323,16 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +351,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -561,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -702,6 +835,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -786,6 +938,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -798,9 +956,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -816,9 +971,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -898,13 +1050,85 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1213,11 +1437,503 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36449082-5C72-4E79-9735-FACEFF87B68B}">
+  <dimension ref="A1:V16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>4</v>
+      </c>
+      <c r="T6">
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <v>4</v>
+      </c>
+      <c r="V6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>5</v>
+      </c>
+      <c r="V7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>6</v>
+      </c>
+      <c r="T8">
+        <v>6</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+      <c r="V8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>7</v>
+      </c>
+      <c r="R9">
+        <v>7</v>
+      </c>
+      <c r="S9">
+        <v>7</v>
+      </c>
+      <c r="T9">
+        <v>7</v>
+      </c>
+      <c r="U9">
+        <v>7</v>
+      </c>
+      <c r="V9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>8</v>
+      </c>
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="T10">
+        <v>8</v>
+      </c>
+      <c r="U10">
+        <v>8</v>
+      </c>
+      <c r="V10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>9</v>
+      </c>
+      <c r="R11">
+        <v>9</v>
+      </c>
+      <c r="S11">
+        <v>9</v>
+      </c>
+      <c r="T11">
+        <v>9</v>
+      </c>
+      <c r="U11">
+        <v>9</v>
+      </c>
+      <c r="V11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB4473A-7175-4429-BDCF-232E357ED7DB}">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39:J39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81:J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,32 +1946,32 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="96" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
       <c r="F2" s="44"/>
-      <c r="G2" s="82" t="s">
+      <c r="G2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="I2" s="82" t="s">
+      <c r="H2" s="105"/>
+      <c r="I2" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="82" t="s">
+      <c r="J2" s="105"/>
+      <c r="K2" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="84"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="89"/>
-      <c r="B3" s="86"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="47"/>
       <c r="D3" s="47"/>
       <c r="E3" s="47"/>
@@ -1280,17 +1996,17 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="72">
+      <c r="A4" s="85">
         <v>1</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="81"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="94"/>
       <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1306,11 +2022,11 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="61"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="74"/>
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1326,11 +2042,11 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="61"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="74"/>
       <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1346,71 +2062,71 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="63"/>
+      <c r="A7" s="85"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="76"/>
       <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="62">
+      <c r="G7" s="75">
         <v>0.45</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="62">
+      <c r="H7" s="76"/>
+      <c r="I7" s="75">
         <v>0.9</v>
       </c>
-      <c r="J7" s="63"/>
+      <c r="J7" s="76"/>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="102" t="s">
+      <c r="A8" s="85"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="117"/>
-      <c r="E8" s="103"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="116"/>
       <c r="F8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="102">
+      <c r="G8" s="115">
         <v>748</v>
       </c>
-      <c r="H8" s="103"/>
-      <c r="I8" s="102">
+      <c r="H8" s="116"/>
+      <c r="I8" s="115">
         <v>19619</v>
       </c>
-      <c r="J8" s="103"/>
+      <c r="J8" s="116"/>
       <c r="K8" s="22"/>
       <c r="L8" s="23"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="63"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="76"/>
       <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="62">
+      <c r="G9" s="75">
         <v>1.7788999999999999</v>
       </c>
-      <c r="H9" s="63"/>
-      <c r="I9" s="62">
+      <c r="H9" s="76"/>
+      <c r="I9" s="75">
         <v>3.6576</v>
       </c>
-      <c r="J9" s="63"/>
+      <c r="J9" s="76"/>
       <c r="K9" s="10"/>
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="100" t="s">
+      <c r="A10" s="85"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="113" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="48"/>
@@ -1418,49 +2134,49 @@
       <c r="F10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="98">
+      <c r="G10" s="102">
         <v>9.6433999999999997</v>
       </c>
-      <c r="H10" s="99"/>
-      <c r="I10" s="98">
+      <c r="H10" s="112"/>
+      <c r="I10" s="102">
         <v>-3.9738000000000002</v>
       </c>
-      <c r="J10" s="99"/>
+      <c r="J10" s="112"/>
       <c r="K10" s="8"/>
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="73"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="101"/>
+      <c r="A11" s="86"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="49"/>
       <c r="E11" s="49"/>
       <c r="F11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="77">
+      <c r="G11" s="90">
         <v>0.4148</v>
       </c>
-      <c r="H11" s="94"/>
-      <c r="I11" s="77">
+      <c r="H11" s="108"/>
+      <c r="I11" s="90">
         <v>1.5122</v>
       </c>
-      <c r="J11" s="94"/>
+      <c r="J11" s="108"/>
       <c r="K11" s="12"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="108">
+      <c r="A12" s="121">
         <v>2</v>
       </c>
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="106"/>
-      <c r="E12" s="120"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="133"/>
       <c r="F12" s="16" t="s">
         <v>5</v>
       </c>
@@ -1478,11 +2194,11 @@
       <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="61"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="74"/>
       <c r="F13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1500,11 +2216,11 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="61"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="74"/>
       <c r="F14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1522,77 +2238,77 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="72"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="63"/>
+      <c r="A15" s="85"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="76"/>
       <c r="F15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="62">
+      <c r="G15" s="75">
         <v>0.45</v>
       </c>
-      <c r="H15" s="63"/>
-      <c r="I15" s="62">
+      <c r="H15" s="76"/>
+      <c r="I15" s="75">
         <v>0.9</v>
       </c>
-      <c r="J15" s="63"/>
-      <c r="K15" s="62">
+      <c r="J15" s="76"/>
+      <c r="K15" s="75">
         <v>0.9</v>
       </c>
-      <c r="L15" s="63"/>
+      <c r="L15" s="76"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="72"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="102" t="s">
+      <c r="A16" s="85"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="117"/>
-      <c r="E16" s="103"/>
+      <c r="D16" s="130"/>
+      <c r="E16" s="116"/>
       <c r="F16" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="102">
+      <c r="G16" s="115">
         <v>1138</v>
       </c>
-      <c r="H16" s="103"/>
-      <c r="I16" s="102">
+      <c r="H16" s="116"/>
+      <c r="I16" s="115">
         <v>19615</v>
       </c>
-      <c r="J16" s="103"/>
-      <c r="K16" s="102">
+      <c r="J16" s="116"/>
+      <c r="K16" s="115">
         <v>49506</v>
       </c>
-      <c r="L16" s="103"/>
+      <c r="L16" s="116"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="72"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="63"/>
+      <c r="A17" s="85"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="76"/>
       <c r="F17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="62">
+      <c r="G17" s="75">
         <v>1.8855999999999999</v>
       </c>
-      <c r="H17" s="63"/>
-      <c r="I17" s="62">
+      <c r="H17" s="76"/>
+      <c r="I17" s="75">
         <v>3.8527999999999998</v>
       </c>
-      <c r="J17" s="63"/>
-      <c r="K17" s="62">
+      <c r="J17" s="76"/>
+      <c r="K17" s="75">
         <v>3.2311999999999999</v>
       </c>
-      <c r="L17" s="63"/>
+      <c r="L17" s="76"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="72"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="107" t="s">
+      <c r="A18" s="85"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="120" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="48"/>
@@ -1600,53 +2316,53 @@
       <c r="F18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="109">
+      <c r="G18" s="122">
         <v>10.0322</v>
       </c>
-      <c r="H18" s="110"/>
-      <c r="I18" s="98">
+      <c r="H18" s="123"/>
+      <c r="I18" s="102">
         <v>8.7571999999999992</v>
       </c>
-      <c r="J18" s="99"/>
-      <c r="K18" s="98">
+      <c r="J18" s="112"/>
+      <c r="K18" s="102">
         <v>2.8107000000000002</v>
       </c>
-      <c r="L18" s="99"/>
+      <c r="L18" s="112"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="73"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="101"/>
+      <c r="A19" s="86"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="114"/>
       <c r="D19" s="49"/>
       <c r="E19" s="49"/>
       <c r="F19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="77">
+      <c r="G19" s="90">
         <v>9.579E-2</v>
       </c>
-      <c r="H19" s="94"/>
-      <c r="I19" s="77">
+      <c r="H19" s="108"/>
+      <c r="I19" s="90">
         <v>0.27729999999999999</v>
       </c>
-      <c r="J19" s="94"/>
-      <c r="K19" s="96">
+      <c r="J19" s="108"/>
+      <c r="K19" s="110">
         <v>-4.0624000000000002</v>
       </c>
-      <c r="L19" s="97"/>
+      <c r="L19" s="111"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="72">
+      <c r="A20" s="85">
         <v>3</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="108" t="s">
+      <c r="C20" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="106"/>
-      <c r="E20" s="120"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="133"/>
       <c r="F20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1662,11 +2378,11 @@
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="72"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="61"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="74"/>
       <c r="F21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1682,11 +2398,11 @@
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="72"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="61"/>
+      <c r="A22" s="85"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="74"/>
       <c r="F22" s="2" t="s">
         <v>7</v>
       </c>
@@ -1702,71 +2418,71 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="72"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="63"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="76"/>
       <c r="F23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="62">
+      <c r="G23" s="75">
         <v>0.45</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="62">
+      <c r="H23" s="76"/>
+      <c r="I23" s="75">
         <v>0.9</v>
       </c>
-      <c r="J23" s="63"/>
+      <c r="J23" s="76"/>
       <c r="K23" s="10"/>
       <c r="L23" s="11"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="72"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="102" t="s">
+      <c r="A24" s="85"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="117"/>
-      <c r="E24" s="103"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="116"/>
       <c r="F24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="102">
+      <c r="G24" s="115">
         <v>418</v>
       </c>
-      <c r="H24" s="103"/>
-      <c r="I24" s="102">
+      <c r="H24" s="116"/>
+      <c r="I24" s="115">
         <v>56607</v>
       </c>
-      <c r="J24" s="103"/>
+      <c r="J24" s="116"/>
       <c r="K24" s="22"/>
       <c r="L24" s="23"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="72"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="63"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="76"/>
       <c r="F25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="62">
+      <c r="G25" s="75">
         <v>3.0828000000000002</v>
       </c>
-      <c r="H25" s="63"/>
-      <c r="I25" s="62">
+      <c r="H25" s="76"/>
+      <c r="I25" s="75">
         <v>3.0446</v>
       </c>
-      <c r="J25" s="63"/>
+      <c r="J25" s="76"/>
       <c r="K25" s="10"/>
       <c r="L25" s="11"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="72"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="107" t="s">
+      <c r="A26" s="85"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="120" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="48"/>
@@ -1774,49 +2490,49 @@
       <c r="F26" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="118">
+      <c r="G26" s="131">
         <v>11.2354</v>
       </c>
-      <c r="H26" s="119"/>
-      <c r="I26" s="98">
+      <c r="H26" s="132"/>
+      <c r="I26" s="102">
         <v>8.9542999999999999</v>
       </c>
-      <c r="J26" s="99"/>
+      <c r="J26" s="112"/>
       <c r="K26" s="8"/>
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="73"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="101"/>
+      <c r="A27" s="86"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="114"/>
       <c r="D27" s="49"/>
       <c r="E27" s="49"/>
       <c r="F27" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="77">
+      <c r="G27" s="90">
         <v>-3.0592000000000001</v>
       </c>
-      <c r="H27" s="94"/>
-      <c r="I27" s="77">
+      <c r="H27" s="108"/>
+      <c r="I27" s="90">
         <v>0.20230000000000001</v>
       </c>
-      <c r="J27" s="94"/>
+      <c r="J27" s="108"/>
       <c r="K27" s="12"/>
       <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="72">
+      <c r="A28" s="85">
         <v>4</v>
       </c>
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="108" t="s">
+      <c r="C28" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="106"/>
-      <c r="E28" s="120"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="133"/>
       <c r="F28" s="2" t="s">
         <v>5</v>
       </c>
@@ -1830,11 +2546,11 @@
       <c r="L28" s="27"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="72"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="61"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="74"/>
       <c r="F29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1848,11 +2564,11 @@
       <c r="L29" s="27"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="72"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="61"/>
+      <c r="A30" s="85"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="74"/>
       <c r="F30" s="2" t="s">
         <v>7</v>
       </c>
@@ -1866,191 +2582,191 @@
       <c r="L30" s="27"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="72"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="63"/>
+      <c r="A31" s="85"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="76"/>
       <c r="F31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="62">
+      <c r="G31" s="75">
         <v>0.95</v>
       </c>
-      <c r="H31" s="63"/>
-      <c r="I31" s="104"/>
-      <c r="J31" s="105"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="117"/>
+      <c r="J31" s="118"/>
       <c r="K31" s="54"/>
       <c r="L31" s="55"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="72"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="102" t="s">
+      <c r="A32" s="85"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="117"/>
-      <c r="E32" s="103"/>
+      <c r="D32" s="130"/>
+      <c r="E32" s="116"/>
       <c r="F32" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="102">
+      <c r="G32" s="115">
         <v>56497</v>
       </c>
-      <c r="H32" s="117"/>
-      <c r="I32" s="113"/>
-      <c r="J32" s="114"/>
+      <c r="H32" s="130"/>
+      <c r="I32" s="126"/>
+      <c r="J32" s="127"/>
       <c r="K32" s="50"/>
       <c r="L32" s="57"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="72"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="63"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="76"/>
       <c r="F33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="62">
+      <c r="G33" s="75">
         <v>1.7931999999999999</v>
       </c>
-      <c r="H33" s="95"/>
-      <c r="I33" s="104"/>
-      <c r="J33" s="105"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="117"/>
+      <c r="J33" s="118"/>
       <c r="K33" s="51"/>
       <c r="L33" s="55"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="72"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="100" t="s">
+      <c r="A34" s="85"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="76" t="s">
+      <c r="D34" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="93"/>
+      <c r="E34" s="107"/>
       <c r="F34" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="111">
+      <c r="G34" s="124">
         <v>9.0103000000000009</v>
       </c>
-      <c r="H34" s="112"/>
-      <c r="I34" s="113"/>
-      <c r="J34" s="114"/>
+      <c r="H34" s="125"/>
+      <c r="I34" s="126"/>
+      <c r="J34" s="127"/>
       <c r="K34" s="56"/>
       <c r="L34" s="57"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="72"/>
-      <c r="B35" s="74"/>
-      <c r="C35" s="107"/>
-      <c r="D35" s="122"/>
-      <c r="E35" s="123"/>
+      <c r="A35" s="85"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="120"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="136"/>
       <c r="F35" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="124">
+      <c r="G35" s="137">
         <v>1.0289999999999999</v>
       </c>
-      <c r="H35" s="125"/>
+      <c r="H35" s="138"/>
       <c r="I35" s="54"/>
       <c r="J35" s="55"/>
       <c r="K35" s="54"/>
       <c r="L35" s="55"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="72"/>
-      <c r="B36" s="74"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="100" t="s">
+      <c r="A36" s="85"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="100" t="s">
+      <c r="E36" s="113" t="s">
         <v>11</v>
       </c>
       <c r="F36" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="111">
+      <c r="G36" s="124">
         <v>0.50480000000000003</v>
       </c>
-      <c r="H36" s="112"/>
+      <c r="H36" s="125"/>
       <c r="I36" s="56"/>
       <c r="J36" s="57"/>
       <c r="K36" s="56"/>
       <c r="L36" s="57"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="72"/>
-      <c r="B37" s="74"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="107"/>
-      <c r="E37" s="121"/>
+      <c r="A37" s="85"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="134"/>
       <c r="F37" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="124">
+      <c r="G37" s="137">
         <v>0.37530000000000002</v>
       </c>
-      <c r="H37" s="125"/>
+      <c r="H37" s="138"/>
       <c r="I37" s="54"/>
       <c r="J37" s="55"/>
       <c r="K37" s="54"/>
       <c r="L37" s="55"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="72"/>
-      <c r="B38" s="74"/>
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="107" t="s">
+      <c r="A38" s="85"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="120" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="111">
+      <c r="G38" s="124">
         <v>0.74819999999999998</v>
       </c>
-      <c r="H38" s="112"/>
+      <c r="H38" s="125"/>
       <c r="I38" s="26"/>
       <c r="J38" s="27"/>
       <c r="K38" s="26"/>
       <c r="L38" s="27"/>
     </row>
     <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="73"/>
-      <c r="B39" s="75"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="101"/>
-      <c r="E39" s="101"/>
+      <c r="A39" s="86"/>
+      <c r="B39" s="88"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="114"/>
+      <c r="E39" s="114"/>
       <c r="F39" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="77">
+      <c r="G39" s="90">
         <v>0.61509999999999998</v>
       </c>
-      <c r="H39" s="94"/>
-      <c r="I39" s="115"/>
-      <c r="J39" s="116"/>
+      <c r="H39" s="108"/>
+      <c r="I39" s="128"/>
+      <c r="J39" s="129"/>
       <c r="K39" s="58"/>
       <c r="L39" s="59"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="72">
+      <c r="A40" s="85">
         <v>5</v>
       </c>
-      <c r="B40" s="74" t="s">
+      <c r="B40" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="108" t="s">
+      <c r="C40" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="106"/>
-      <c r="E40" s="120"/>
+      <c r="D40" s="119"/>
+      <c r="E40" s="133"/>
       <c r="F40" s="2" t="s">
         <v>5</v>
       </c>
@@ -2064,11 +2780,11 @@
       <c r="L40" s="9"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="72"/>
-      <c r="B41" s="74"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="61"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="87"/>
+      <c r="E41" s="74"/>
       <c r="F41" s="2" t="s">
         <v>6</v>
       </c>
@@ -2082,11 +2798,11 @@
       <c r="L41" s="9"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="72"/>
-      <c r="B42" s="74"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="61"/>
+      <c r="A42" s="85"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="85"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="74"/>
       <c r="F42" s="2" t="s">
         <v>7</v>
       </c>
@@ -2100,204 +2816,204 @@
       <c r="L42" s="9"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="72"/>
-      <c r="B43" s="74"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="95"/>
-      <c r="E43" s="63"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="109"/>
+      <c r="E43" s="76"/>
       <c r="F43" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="62">
+      <c r="G43" s="75">
         <v>0.95</v>
       </c>
-      <c r="H43" s="63"/>
-      <c r="I43" s="104"/>
-      <c r="J43" s="105"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="117"/>
+      <c r="J43" s="118"/>
       <c r="K43" s="10"/>
       <c r="L43" s="11"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="72"/>
-      <c r="B44" s="74"/>
-      <c r="C44" s="102" t="s">
+      <c r="A44" s="85"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="117"/>
-      <c r="E44" s="103"/>
+      <c r="D44" s="130"/>
+      <c r="E44" s="116"/>
       <c r="F44" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="102">
+      <c r="G44" s="115">
         <v>58601</v>
       </c>
-      <c r="H44" s="117"/>
-      <c r="I44" s="113"/>
-      <c r="J44" s="114"/>
+      <c r="H44" s="130"/>
+      <c r="I44" s="126"/>
+      <c r="J44" s="127"/>
       <c r="K44" s="50"/>
       <c r="L44" s="23"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="72"/>
-      <c r="B45" s="74"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="95"/>
-      <c r="E45" s="63"/>
+      <c r="A45" s="85"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="109"/>
+      <c r="E45" s="76"/>
       <c r="F45" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G45" s="62">
+      <c r="G45" s="75">
         <v>1.7312000000000001</v>
       </c>
-      <c r="H45" s="95"/>
-      <c r="I45" s="104"/>
-      <c r="J45" s="105"/>
+      <c r="H45" s="109"/>
+      <c r="I45" s="117"/>
+      <c r="J45" s="118"/>
       <c r="K45" s="51"/>
       <c r="L45" s="11"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="72"/>
-      <c r="B46" s="74"/>
-      <c r="C46" s="100" t="s">
+      <c r="A46" s="85"/>
+      <c r="B46" s="87"/>
+      <c r="C46" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="76" t="s">
+      <c r="D46" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="E46" s="93"/>
+      <c r="E46" s="107"/>
       <c r="F46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="111">
+      <c r="G46" s="124">
         <v>2.5280999999999998</v>
       </c>
-      <c r="H46" s="112"/>
-      <c r="I46" s="113"/>
-      <c r="J46" s="114"/>
+      <c r="H46" s="125"/>
+      <c r="I46" s="126"/>
+      <c r="J46" s="127"/>
       <c r="K46" s="22"/>
       <c r="L46" s="23"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="72"/>
-      <c r="B47" s="74"/>
-      <c r="C47" s="107"/>
-      <c r="D47" s="122"/>
-      <c r="E47" s="123"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="87"/>
+      <c r="C47" s="120"/>
+      <c r="D47" s="135"/>
+      <c r="E47" s="136"/>
       <c r="F47" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G47" s="124">
+      <c r="G47" s="137">
         <v>-3.6394000000000002</v>
       </c>
-      <c r="H47" s="125"/>
+      <c r="H47" s="138"/>
       <c r="I47" s="24"/>
       <c r="J47" s="25"/>
       <c r="K47" s="24"/>
       <c r="L47" s="25"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="72"/>
-      <c r="B48" s="74"/>
-      <c r="C48" s="107"/>
-      <c r="D48" s="100" t="s">
+      <c r="A48" s="85"/>
+      <c r="B48" s="87"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="100" t="s">
+      <c r="E48" s="113" t="s">
         <v>11</v>
       </c>
       <c r="F48" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G48" s="111">
+      <c r="G48" s="124">
         <v>0.32040000000000002</v>
       </c>
-      <c r="H48" s="112"/>
+      <c r="H48" s="125"/>
       <c r="I48" s="22"/>
       <c r="J48" s="23"/>
       <c r="K48" s="22"/>
       <c r="L48" s="23"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="72"/>
-      <c r="B49" s="74"/>
-      <c r="C49" s="107"/>
-      <c r="D49" s="107"/>
-      <c r="E49" s="121"/>
+      <c r="A49" s="85"/>
+      <c r="B49" s="87"/>
+      <c r="C49" s="120"/>
+      <c r="D49" s="120"/>
+      <c r="E49" s="134"/>
       <c r="F49" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="G49" s="124"/>
-      <c r="H49" s="125"/>
+      <c r="G49" s="137"/>
+      <c r="H49" s="138"/>
       <c r="I49" s="24"/>
       <c r="J49" s="25"/>
       <c r="K49" s="24"/>
       <c r="L49" s="25"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="72"/>
-      <c r="B50" s="74"/>
-      <c r="C50" s="107"/>
-      <c r="D50" s="107"/>
-      <c r="E50" s="107" t="s">
+      <c r="A50" s="85"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="120"/>
+      <c r="D50" s="120"/>
+      <c r="E50" s="120" t="s">
         <v>12</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G50" s="111">
+      <c r="G50" s="124">
         <v>0.62639999999999996</v>
       </c>
-      <c r="H50" s="112"/>
+      <c r="H50" s="125"/>
       <c r="I50" s="26"/>
       <c r="J50" s="27"/>
       <c r="K50" s="26"/>
       <c r="L50" s="27"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="73"/>
-      <c r="B51" s="75"/>
-      <c r="C51" s="101"/>
-      <c r="D51" s="101"/>
-      <c r="E51" s="101"/>
+      <c r="A51" s="86"/>
+      <c r="B51" s="88"/>
+      <c r="C51" s="114"/>
+      <c r="D51" s="114"/>
+      <c r="E51" s="114"/>
       <c r="F51" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="77"/>
-      <c r="H51" s="94"/>
-      <c r="I51" s="115"/>
-      <c r="J51" s="116"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="108"/>
+      <c r="I51" s="128"/>
+      <c r="J51" s="129"/>
       <c r="K51" s="12"/>
       <c r="L51" s="13"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="88" t="s">
+      <c r="A55" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="83" t="s">
+      <c r="B55" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="82"/>
+      <c r="C55" s="95"/>
       <c r="D55" s="28"/>
       <c r="E55" s="28"/>
-      <c r="F55" s="90"/>
-      <c r="G55" s="82" t="s">
+      <c r="F55" s="105"/>
+      <c r="G55" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="H55" s="84"/>
+      <c r="H55" s="97"/>
       <c r="I55" s="34"/>
       <c r="J55" s="32"/>
       <c r="K55" s="32"/>
       <c r="L55" s="32"/>
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="89"/>
-      <c r="B56" s="86"/>
-      <c r="C56" s="85"/>
+      <c r="A56" s="104"/>
+      <c r="B56" s="99"/>
+      <c r="C56" s="98"/>
       <c r="D56" s="29"/>
       <c r="E56" s="29"/>
-      <c r="F56" s="91"/>
+      <c r="F56" s="106"/>
       <c r="G56" s="4" t="s">
         <v>1</v>
       </c>
@@ -2310,17 +3026,17 @@
       <c r="L56" s="32"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="80">
+      <c r="A57" s="93">
         <v>1</v>
       </c>
-      <c r="B57" s="92" t="s">
+      <c r="B57" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="C57" s="80" t="s">
+      <c r="C57" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="D57" s="92"/>
-      <c r="E57" s="92"/>
+      <c r="D57" s="101"/>
+      <c r="E57" s="101"/>
       <c r="F57" s="36" t="s">
         <v>5</v>
       </c>
@@ -2334,11 +3050,11 @@
       <c r="L57" s="32"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="72"/>
-      <c r="B58" s="74"/>
-      <c r="C58" s="72"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
+      <c r="A58" s="85"/>
+      <c r="B58" s="87"/>
+      <c r="C58" s="85"/>
+      <c r="D58" s="87"/>
+      <c r="E58" s="87"/>
       <c r="F58" s="2" t="s">
         <v>6</v>
       </c>
@@ -2352,11 +3068,11 @@
       <c r="L58" s="32"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="72"/>
-      <c r="B59" s="74"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="95"/>
-      <c r="E59" s="95"/>
+      <c r="A59" s="85"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="109"/>
+      <c r="E59" s="109"/>
       <c r="F59" s="2" t="s">
         <v>21</v>
       </c>
@@ -2370,9 +3086,9 @@
       <c r="L59" s="32"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="72"/>
-      <c r="B60" s="74"/>
-      <c r="C60" s="76" t="s">
+      <c r="A60" s="85"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="89" t="s">
         <v>10</v>
       </c>
       <c r="D60" s="40"/>
@@ -2380,45 +3096,45 @@
       <c r="F60" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G60" s="76">
+      <c r="G60" s="89">
         <v>6.3207000000000004</v>
       </c>
-      <c r="H60" s="93"/>
+      <c r="H60" s="107"/>
       <c r="I60" s="33"/>
       <c r="J60" s="32"/>
       <c r="K60" s="32"/>
       <c r="L60" s="32"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="73"/>
-      <c r="B61" s="75"/>
-      <c r="C61" s="77"/>
+      <c r="A61" s="86"/>
+      <c r="B61" s="88"/>
+      <c r="C61" s="90"/>
       <c r="D61" s="39"/>
       <c r="E61" s="39"/>
       <c r="F61" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G61" s="77">
+      <c r="G61" s="90">
         <v>-2.7806999999999999</v>
       </c>
-      <c r="H61" s="94"/>
+      <c r="H61" s="108"/>
       <c r="I61" s="33"/>
       <c r="J61" s="32"/>
       <c r="K61" s="32"/>
       <c r="L61" s="32"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="72">
+      <c r="A62" s="85">
         <v>2</v>
       </c>
-      <c r="B62" s="74" t="s">
+      <c r="B62" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="108" t="s">
+      <c r="C62" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="106"/>
-      <c r="E62" s="106"/>
+      <c r="D62" s="119"/>
+      <c r="E62" s="119"/>
       <c r="F62" s="2" t="s">
         <v>5</v>
       </c>
@@ -2432,11 +3148,11 @@
       <c r="L62" s="32"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="72"/>
-      <c r="B63" s="74"/>
-      <c r="C63" s="72"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
+      <c r="A63" s="85"/>
+      <c r="B63" s="87"/>
+      <c r="C63" s="85"/>
+      <c r="D63" s="87"/>
+      <c r="E63" s="87"/>
       <c r="F63" s="2" t="s">
         <v>6</v>
       </c>
@@ -2450,11 +3166,11 @@
       <c r="L63" s="32"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="72"/>
-      <c r="B64" s="74"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="95"/>
-      <c r="E64" s="95"/>
+      <c r="A64" s="85"/>
+      <c r="B64" s="87"/>
+      <c r="C64" s="75"/>
+      <c r="D64" s="109"/>
+      <c r="E64" s="109"/>
       <c r="F64" s="2" t="s">
         <v>21</v>
       </c>
@@ -2468,9 +3184,9 @@
       <c r="L64" s="32"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="72"/>
-      <c r="B65" s="74"/>
-      <c r="C65" s="76" t="s">
+      <c r="A65" s="85"/>
+      <c r="B65" s="87"/>
+      <c r="C65" s="89" t="s">
         <v>10</v>
       </c>
       <c r="D65" s="40"/>
@@ -2478,28 +3194,28 @@
       <c r="F65" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G65" s="78">
+      <c r="G65" s="91">
         <v>10.9224</v>
       </c>
-      <c r="H65" s="79"/>
+      <c r="H65" s="92"/>
       <c r="I65" s="33"/>
       <c r="J65" s="32"/>
       <c r="K65" s="32"/>
       <c r="L65" s="32"/>
     </row>
     <row r="66" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="73"/>
-      <c r="B66" s="75"/>
-      <c r="C66" s="77"/>
+      <c r="A66" s="86"/>
+      <c r="B66" s="88"/>
+      <c r="C66" s="90"/>
       <c r="D66" s="39"/>
       <c r="E66" s="39"/>
       <c r="F66" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G66" s="77">
+      <c r="G66" s="90">
         <v>-1.8394999999999999</v>
       </c>
-      <c r="H66" s="94"/>
+      <c r="H66" s="108"/>
       <c r="I66" s="33"/>
       <c r="J66" s="32"/>
       <c r="K66" s="32"/>
@@ -2508,300 +3224,300 @@
     <row r="67" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="88" t="s">
+      <c r="A70" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="83" t="s">
+      <c r="B70" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="82"/>
+      <c r="C70" s="95"/>
       <c r="D70" s="42"/>
       <c r="E70" s="30"/>
-      <c r="F70" s="90"/>
-      <c r="G70" s="82" t="s">
+      <c r="F70" s="105"/>
+      <c r="G70" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="H70" s="83"/>
-      <c r="I70" s="83"/>
-      <c r="J70" s="84"/>
+      <c r="H70" s="96"/>
+      <c r="I70" s="96"/>
+      <c r="J70" s="97"/>
     </row>
     <row r="71" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="89"/>
-      <c r="B71" s="86"/>
-      <c r="C71" s="85"/>
+      <c r="A71" s="104"/>
+      <c r="B71" s="99"/>
+      <c r="C71" s="98"/>
       <c r="D71" s="41"/>
       <c r="E71" s="31"/>
-      <c r="F71" s="91"/>
-      <c r="G71" s="85" t="s">
+      <c r="F71" s="106"/>
+      <c r="G71" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="H71" s="86"/>
-      <c r="I71" s="86"/>
-      <c r="J71" s="87"/>
+      <c r="H71" s="99"/>
+      <c r="I71" s="99"/>
+      <c r="J71" s="100"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="80">
+      <c r="A72" s="93">
         <v>1</v>
       </c>
-      <c r="B72" s="92" t="s">
+      <c r="B72" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="C72" s="80" t="s">
+      <c r="C72" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="D72" s="92"/>
-      <c r="E72" s="81"/>
+      <c r="D72" s="101"/>
+      <c r="E72" s="94"/>
       <c r="F72" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G72" s="80" t="s">
+      <c r="G72" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="H72" s="81"/>
-      <c r="I72" s="80" t="s">
+      <c r="H72" s="94"/>
+      <c r="I72" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="J72" s="81"/>
+      <c r="J72" s="94"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="72"/>
-      <c r="B73" s="74"/>
-      <c r="C73" s="72"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="61"/>
+      <c r="A73" s="85"/>
+      <c r="B73" s="87"/>
+      <c r="C73" s="85"/>
+      <c r="D73" s="87"/>
+      <c r="E73" s="74"/>
       <c r="F73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G73" s="72" t="s">
+      <c r="G73" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="H73" s="61"/>
-      <c r="I73" s="72" t="s">
+      <c r="H73" s="74"/>
+      <c r="I73" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="J73" s="61"/>
+      <c r="J73" s="74"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="72"/>
-      <c r="B74" s="74"/>
-      <c r="C74" s="72"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="61"/>
+      <c r="A74" s="85"/>
+      <c r="B74" s="87"/>
+      <c r="C74" s="85"/>
+      <c r="D74" s="87"/>
+      <c r="E74" s="74"/>
       <c r="F74" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G74" s="72">
+      <c r="G74" s="85">
         <v>7</v>
       </c>
-      <c r="H74" s="61"/>
-      <c r="I74" s="72">
+      <c r="H74" s="74"/>
+      <c r="I74" s="85">
         <v>10</v>
       </c>
-      <c r="J74" s="61"/>
+      <c r="J74" s="74"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="72"/>
-      <c r="B75" s="74"/>
-      <c r="C75" s="72"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="61"/>
+      <c r="A75" s="85"/>
+      <c r="B75" s="87"/>
+      <c r="C75" s="85"/>
+      <c r="D75" s="87"/>
+      <c r="E75" s="74"/>
       <c r="F75" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G75" s="60" t="s">
+      <c r="G75" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="H75" s="61"/>
-      <c r="I75" s="60" t="s">
+      <c r="H75" s="74"/>
+      <c r="I75" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="J75" s="61"/>
+      <c r="J75" s="74"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="72"/>
-      <c r="B76" s="74"/>
-      <c r="C76" s="72"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="61"/>
+      <c r="A76" s="85"/>
+      <c r="B76" s="87"/>
+      <c r="C76" s="85"/>
+      <c r="D76" s="87"/>
+      <c r="E76" s="74"/>
       <c r="F76" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G76" s="60" t="s">
+      <c r="G76" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="H76" s="61"/>
-      <c r="I76" s="60" t="s">
+      <c r="H76" s="74"/>
+      <c r="I76" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="J76" s="61"/>
+      <c r="J76" s="74"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="72"/>
-      <c r="B77" s="74"/>
-      <c r="C77" s="62"/>
-      <c r="D77" s="95"/>
-      <c r="E77" s="63"/>
+      <c r="A77" s="85"/>
+      <c r="B77" s="87"/>
+      <c r="C77" s="75"/>
+      <c r="D77" s="109"/>
+      <c r="E77" s="76"/>
       <c r="F77" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G77" s="62">
+      <c r="G77" s="75">
         <v>50</v>
       </c>
-      <c r="H77" s="63"/>
-      <c r="I77" s="62">
+      <c r="H77" s="76"/>
+      <c r="I77" s="75">
         <v>50</v>
       </c>
-      <c r="J77" s="63"/>
+      <c r="J77" s="76"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="72"/>
-      <c r="B78" s="74"/>
-      <c r="C78" s="76" t="s">
+      <c r="A78" s="85"/>
+      <c r="B78" s="87"/>
+      <c r="C78" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="D78" s="76" t="s">
+      <c r="D78" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="E78" s="93"/>
+      <c r="E78" s="107"/>
       <c r="F78" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G78" s="64">
+      <c r="G78" s="77">
         <v>8.5784000000000002</v>
       </c>
-      <c r="H78" s="65"/>
-      <c r="I78" s="64">
+      <c r="H78" s="78"/>
+      <c r="I78" s="77">
         <v>8.1113999999999997</v>
       </c>
-      <c r="J78" s="65"/>
+      <c r="J78" s="78"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="72"/>
-      <c r="B79" s="74"/>
-      <c r="C79" s="98"/>
-      <c r="D79" s="122"/>
-      <c r="E79" s="123"/>
+      <c r="A79" s="85"/>
+      <c r="B79" s="87"/>
+      <c r="C79" s="102"/>
+      <c r="D79" s="135"/>
+      <c r="E79" s="136"/>
       <c r="F79" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G79" s="66">
+      <c r="G79" s="79">
         <v>-1.1739999999999999</v>
       </c>
-      <c r="H79" s="67"/>
-      <c r="I79" s="66">
+      <c r="H79" s="80"/>
+      <c r="I79" s="79">
         <v>-1.0732999999999999</v>
       </c>
-      <c r="J79" s="67"/>
+      <c r="J79" s="80"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="72"/>
-      <c r="B80" s="74"/>
-      <c r="C80" s="98"/>
-      <c r="D80" s="107" t="s">
+      <c r="A80" s="85"/>
+      <c r="B80" s="87"/>
+      <c r="C80" s="102"/>
+      <c r="D80" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="E80" s="100" t="s">
+      <c r="E80" s="113" t="s">
         <v>11</v>
       </c>
       <c r="F80" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G80" s="64">
+      <c r="G80" s="77">
         <v>0.9355</v>
       </c>
-      <c r="H80" s="65"/>
-      <c r="I80" s="64">
+      <c r="H80" s="78"/>
+      <c r="I80" s="77">
         <v>0.93600000000000005</v>
       </c>
-      <c r="J80" s="65"/>
+      <c r="J80" s="78"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="72"/>
-      <c r="B81" s="74"/>
-      <c r="C81" s="98"/>
-      <c r="D81" s="107"/>
-      <c r="E81" s="107"/>
+      <c r="A81" s="85"/>
+      <c r="B81" s="87"/>
+      <c r="C81" s="102"/>
+      <c r="D81" s="120"/>
+      <c r="E81" s="120"/>
       <c r="F81" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G81" s="68">
+      <c r="G81" s="81">
         <v>0.93240000000000001</v>
       </c>
-      <c r="H81" s="69"/>
-      <c r="I81" s="68">
+      <c r="H81" s="82"/>
+      <c r="I81" s="81">
         <v>0.93330000000000002</v>
       </c>
-      <c r="J81" s="69"/>
+      <c r="J81" s="82"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="72"/>
-      <c r="B82" s="74"/>
-      <c r="C82" s="98"/>
-      <c r="D82" s="107"/>
-      <c r="E82" s="121"/>
+      <c r="A82" s="85"/>
+      <c r="B82" s="87"/>
+      <c r="C82" s="102"/>
+      <c r="D82" s="120"/>
+      <c r="E82" s="134"/>
       <c r="F82" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="G82" s="66"/>
-      <c r="H82" s="67"/>
-      <c r="I82" s="66" t="s">
+      <c r="G82" s="79"/>
+      <c r="H82" s="80"/>
+      <c r="I82" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="J82" s="67"/>
+      <c r="J82" s="80"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="72"/>
-      <c r="B83" s="74"/>
-      <c r="C83" s="98"/>
-      <c r="D83" s="107"/>
-      <c r="E83" s="107" t="s">
+      <c r="A83" s="85"/>
+      <c r="B83" s="87"/>
+      <c r="C83" s="102"/>
+      <c r="D83" s="120"/>
+      <c r="E83" s="120" t="s">
         <v>12</v>
       </c>
       <c r="F83" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G83" s="68">
+      <c r="G83" s="81">
         <v>0.9486</v>
       </c>
-      <c r="H83" s="69"/>
-      <c r="I83" s="68">
+      <c r="H83" s="82"/>
+      <c r="I83" s="81">
         <v>0.94889999999999997</v>
       </c>
-      <c r="J83" s="69"/>
+      <c r="J83" s="82"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="72"/>
-      <c r="B84" s="74"/>
-      <c r="C84" s="98"/>
-      <c r="D84" s="107"/>
-      <c r="E84" s="107"/>
+      <c r="A84" s="85"/>
+      <c r="B84" s="87"/>
+      <c r="C84" s="102"/>
+      <c r="D84" s="120"/>
+      <c r="E84" s="120"/>
       <c r="F84" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G84" s="68">
+      <c r="G84" s="81">
         <v>0.94399999999999995</v>
       </c>
-      <c r="H84" s="69"/>
-      <c r="I84" s="68">
+      <c r="H84" s="82"/>
+      <c r="I84" s="81">
         <v>0.94499999999999995</v>
       </c>
-      <c r="J84" s="69"/>
+      <c r="J84" s="82"/>
     </row>
     <row r="85" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="73"/>
-      <c r="B85" s="75"/>
-      <c r="C85" s="77"/>
-      <c r="D85" s="101"/>
-      <c r="E85" s="101"/>
+      <c r="A85" s="86"/>
+      <c r="B85" s="88"/>
+      <c r="C85" s="90"/>
+      <c r="D85" s="114"/>
+      <c r="E85" s="114"/>
       <c r="F85" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G85" s="70"/>
-      <c r="H85" s="71"/>
-      <c r="I85" s="70" t="s">
+      <c r="G85" s="83"/>
+      <c r="H85" s="84"/>
+      <c r="I85" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="J85" s="71"/>
+      <c r="J85" s="84"/>
     </row>
     <row r="86" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2970,4 +3686,188 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA02051B-5D8B-422C-AB61-3ADFBE2D2369}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" style="60" customWidth="1"/>
+    <col min="2" max="9" width="16.7109375" style="72" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="141" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="139" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="140"/>
+      <c r="D1" s="139" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="143"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="139" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="143"/>
+      <c r="I1" s="140"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="142"/>
+      <c r="B2" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="62" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="65">
+        <v>-6.1037521730897799</v>
+      </c>
+      <c r="C3" s="66">
+        <v>0.26916882532647002</v>
+      </c>
+      <c r="D3" s="67">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="E3" s="67">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="F3" s="67">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="G3" s="65">
+        <v>0.394736842105263</v>
+      </c>
+      <c r="H3" s="67">
+        <v>0.18269230769230699</v>
+      </c>
+      <c r="I3" s="66">
+        <v>0.25776397515527899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="65">
+        <v>9.0103079149248995</v>
+      </c>
+      <c r="C4" s="66">
+        <v>1.02898829850197</v>
+      </c>
+      <c r="D4" s="67">
+        <v>0.90571428571428503</v>
+      </c>
+      <c r="E4" s="67">
+        <v>0.95714285714285696</v>
+      </c>
+      <c r="F4" s="67">
+        <v>0.84428571428571397</v>
+      </c>
+      <c r="G4" s="65">
+        <v>0.49122807017543801</v>
+      </c>
+      <c r="H4" s="67">
+        <v>0.18269230769230699</v>
+      </c>
+      <c r="I4" s="66">
+        <v>0.467391304347826</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="69">
+        <v>8.2532112514673894</v>
+      </c>
+      <c r="C5" s="70">
+        <v>-4.9804476659040904E-3</v>
+      </c>
+      <c r="D5" s="71">
+        <v>0.66</v>
+      </c>
+      <c r="E5" s="71">
+        <v>0.71</v>
+      </c>
+      <c r="F5" s="71">
+        <v>0.64571428571428502</v>
+      </c>
+      <c r="G5" s="69">
+        <v>0.52631578947368396</v>
+      </c>
+      <c r="H5" s="71">
+        <v>0.51442307692307598</v>
+      </c>
+      <c r="I5" s="70">
+        <v>0.51863354037266995</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="top10" dxfId="7" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="top10" dxfId="6" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="top10" dxfId="5" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="top10" dxfId="4" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>